<commit_message>
[PCB]: components arrangment around 3 MOSFET drivers
</commit_message>
<xml_diff>
--- a/bom.xlsx
+++ b/bom.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t xml:space="preserve">компонент</t>
   </si>
@@ -71,6 +71,12 @@
   </si>
   <si>
     <t xml:space="preserve">https://belchip.by/product/?selected_product=18408</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Коннектор</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://belchip.by/product/?selected_product=38607</t>
   </si>
 </sst>
 </file>
@@ -108,6 +114,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -402,7 +409,15 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C9" s="2"/>
+      <c r="A9" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="11" customFormat="false" ht="81" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>